<commit_message>
Update 1. Final Project Management.xlsx
</commit_message>
<xml_diff>
--- a/Documents/1. Final Project Management.xlsx
+++ b/Documents/1. Final Project Management.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{34DA8DFC-7E4C-426E-9A80-A4A754AC0F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00976019-73B0-4A99-AA0E-47CD2126735C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F83083-930B-4CEB-AD12-639E09FE90C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -890,23 +890,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1476,9 +1476,9 @@
   </sheetPr>
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1504,9 @@
     <col min="23" max="23" width="3.140625" customWidth="1"/>
     <col min="24" max="25" width="3.85546875" customWidth="1"/>
     <col min="26" max="26" width="3.42578125" customWidth="1"/>
-    <col min="27" max="64" width="2.5703125" customWidth="1"/>
+    <col min="27" max="50" width="2.5703125" customWidth="1"/>
+    <col min="51" max="51" width="4.28515625" customWidth="1"/>
+    <col min="52" max="64" width="2.5703125" customWidth="1"/>
     <col min="69" max="70" width="10.28515625"/>
   </cols>
   <sheetData>
@@ -1542,106 +1544,106 @@
       <c r="B3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="89">
+      <c r="D3" s="89"/>
+      <c r="E3" s="87">
         <v>44999</v>
       </c>
-      <c r="F3" s="89"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="84">
         <f>I5</f>
         <v>44998</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="84">
         <f>P5</f>
         <v>45005</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="84">
         <f>W5</f>
         <v>45012</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="84">
         <f>AD5</f>
         <v>45019</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="84">
         <f>AK5</f>
         <v>45026</v>
       </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="85"/>
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="86"/>
+      <c r="AR4" s="84">
         <f>AR5</f>
         <v>45033</v>
       </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="85"/>
+      <c r="AW4" s="85"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="84">
         <f>AY5</f>
         <v>45040</v>
       </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+      <c r="AZ4" s="85"/>
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="85"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="84">
         <f>BF5</f>
         <v>45047</v>
       </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
@@ -4572,17 +4574,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D38">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
Delete and Create new project folder
</commit_message>
<xml_diff>
--- a/Documents/1. Final Project Management.xlsx
+++ b/Documents/1. Final Project Management.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD44EFA9-C56F-43B5-B82A-B6DA11C7086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2260B4-3D10-4798-A354-AD96D9FAA3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="720" windowWidth="24615" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -890,6 +890,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -901,12 +907,6 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1476,9 +1476,9 @@
   </sheetPr>
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN29" sqref="AN29"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AR30" sqref="AR30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1547,106 +1547,106 @@
       <c r="B3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="87">
+      <c r="D3" s="85"/>
+      <c r="E3" s="89">
         <v>44999</v>
       </c>
-      <c r="F3" s="87"/>
+      <c r="F3" s="89"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="84">
+      <c r="I4" s="86">
         <f>I5</f>
         <v>44998</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="84">
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86">
         <f>P5</f>
         <v>45005</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="84">
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86">
         <f>W5</f>
         <v>45012</v>
       </c>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="84">
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86">
         <f>AD5</f>
         <v>45019</v>
       </c>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="84">
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="86">
         <f>AK5</f>
         <v>45026</v>
       </c>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="85"/>
-      <c r="AO4" s="85"/>
-      <c r="AP4" s="85"/>
-      <c r="AQ4" s="86"/>
-      <c r="AR4" s="84">
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="87"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="87"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="86">
         <f>AR5</f>
         <v>45033</v>
       </c>
-      <c r="AS4" s="85"/>
-      <c r="AT4" s="85"/>
-      <c r="AU4" s="85"/>
-      <c r="AV4" s="85"/>
-      <c r="AW4" s="85"/>
-      <c r="AX4" s="86"/>
-      <c r="AY4" s="84">
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="87"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="86">
         <f>AY5</f>
         <v>45040</v>
       </c>
-      <c r="AZ4" s="85"/>
-      <c r="BA4" s="85"/>
-      <c r="BB4" s="85"/>
-      <c r="BC4" s="85"/>
-      <c r="BD4" s="85"/>
-      <c r="BE4" s="86"/>
-      <c r="BF4" s="84">
+      <c r="AZ4" s="87"/>
+      <c r="BA4" s="87"/>
+      <c r="BB4" s="87"/>
+      <c r="BC4" s="87"/>
+      <c r="BD4" s="87"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="86">
         <f>BF5</f>
         <v>45047</v>
       </c>
-      <c r="BG4" s="85"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="85"/>
-      <c r="BJ4" s="85"/>
-      <c r="BK4" s="85"/>
-      <c r="BL4" s="86"/>
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="87"/>
+      <c r="BI4" s="87"/>
+      <c r="BJ4" s="87"/>
+      <c r="BK4" s="87"/>
+      <c r="BL4" s="88"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
@@ -4577,17 +4577,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D38">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
Big Boss and UIHealthBar
</commit_message>
<xml_diff>
--- a/Documents/1. Final Project Management.xlsx
+++ b/Documents/1. Final Project Management.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2260B4-3D10-4798-A354-AD96D9FAA3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D880D3FF-335D-402F-893D-691B302ADC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="720" windowWidth="24615" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,23 +890,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1476,8 +1476,8 @@
   </sheetPr>
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AR30" sqref="AR30"/>
     </sheetView>
   </sheetViews>
@@ -1547,106 +1547,106 @@
       <c r="B3" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="89">
+      <c r="D3" s="89"/>
+      <c r="E3" s="87">
         <v>44999</v>
       </c>
-      <c r="F3" s="89"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="84">
         <f>I5</f>
         <v>44998</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="84">
         <f>P5</f>
         <v>45005</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="84">
         <f>W5</f>
         <v>45012</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="84">
         <f>AD5</f>
         <v>45019</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="84">
         <f>AK5</f>
         <v>45026</v>
       </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+      <c r="AL4" s="85"/>
+      <c r="AM4" s="85"/>
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="85"/>
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="86"/>
+      <c r="AR4" s="84">
         <f>AR5</f>
         <v>45033</v>
       </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+      <c r="AS4" s="85"/>
+      <c r="AT4" s="85"/>
+      <c r="AU4" s="85"/>
+      <c r="AV4" s="85"/>
+      <c r="AW4" s="85"/>
+      <c r="AX4" s="86"/>
+      <c r="AY4" s="84">
         <f>AY5</f>
         <v>45040</v>
       </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+      <c r="AZ4" s="85"/>
+      <c r="BA4" s="85"/>
+      <c r="BB4" s="85"/>
+      <c r="BC4" s="85"/>
+      <c r="BD4" s="85"/>
+      <c r="BE4" s="86"/>
+      <c r="BF4" s="84">
         <f>BF5</f>
         <v>45047</v>
       </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="85"/>
+      <c r="BI4" s="85"/>
+      <c r="BJ4" s="85"/>
+      <c r="BK4" s="85"/>
+      <c r="BL4" s="86"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
@@ -4577,17 +4577,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D38">
     <cfRule type="dataBar" priority="14">

</xml_diff>